<commit_message>
MALS-1119 Update apiary inspection template
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Apiary_Hive_Inspection_Template.xlsx
+++ b/app/server/static/templates/reports/Apiary_Hive_Inspection_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1011A04A-70C7-4033-80DA-166118876B8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56012DB2-1FFB-4760-823F-865C09DE886A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>Last Name</t>
   </si>
@@ -240,9 +240,6 @@
     <t>{d.Tot_EFB}</t>
   </si>
   <si>
-    <t>{d.TotNosema}</t>
-  </si>
-  <si>
     <t>{d.Tot_Chalkbrood}</t>
   </si>
   <si>
@@ -268,6 +265,18 @@
   </si>
   <si>
     <t>Date &amp; Time Report Created (UTC)</t>
+  </si>
+  <si>
+    <t>{d.Tot_Broods_Inspected}</t>
+  </si>
+  <si>
+    <t>{d.Tot_Nosema}</t>
+  </si>
+  <si>
+    <t>Colonies Inspected Brood</t>
+  </si>
+  <si>
+    <t>{d.Region[i].BroodsInspected}</t>
   </si>
 </sst>
 </file>
@@ -916,49 +925,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB249F7-276C-4CD0-823C-DE856519B24C}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
-    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="11"/>
       <c r="E1" s="11"/>
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="N1" s="12" t="s">
+      <c r="K1" s="11"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O1" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="11"/>
       <c r="C2" s="11" t="s">
@@ -973,26 +983,28 @@
       <c r="F2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="11"/>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
       <c r="J2" s="11"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K2" s="11"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
@@ -1000,101 +1012,108 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="F6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="J6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="J7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="M7" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="N7" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="8"/>
       <c r="F11" s="10"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="8"/>
+      <c r="H11" s="10"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
-      <c r="K11" s="10"/>
+      <c r="K11" s="8"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -1108,8 +1127,9 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1117,37 +1137,40 @@
         <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1157,21 +1180,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fc8a81a77eeb73bda9729b3f784b8c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88ad40c7f0e134defa4acd5e486d3459" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1382,32 +1390,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8385E0-3C6B-44E0-B051-89C807FA11B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D213D4AC-AA3E-4F07-BD45-2E303A245682}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{710596F7-33DB-499C-9202-13CC66DA1061}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1424,4 +1422,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D213D4AC-AA3E-4F07-BD45-2E303A245682}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8385E0-3C6B-44E0-B051-89C807FA11B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add columns to report
</commit_message>
<xml_diff>
--- a/app/server/static/templates/reports/Apiary_Hive_Inspection_Template.xlsx
+++ b/app/server/static/templates/reports/Apiary_Hive_Inspection_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\MALS\app\server\static\templates\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gh\nr-mals\app\server\static\templates\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56012DB2-1FFB-4760-823F-865C09DE886A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2C860E-C4C2-4FF8-BAD8-FFCCAA82516A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
+    <workbookView xWindow="41220" yWindow="840" windowWidth="32025" windowHeight="15345" xr2:uid="{11309506-049F-4A42-8D72-2555D662D497}"/>
   </bookViews>
   <sheets>
     <sheet name="Apiary Hive Inspection" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Last Name</t>
   </si>
@@ -186,9 +186,6 @@
     <t>{d.Licence[i].TotalNumHives}</t>
   </si>
   <si>
-    <t>{d.Licence[i+1].LicenceNumber}</t>
-  </si>
-  <si>
     <t>{d.Region[i].RegionName}</t>
   </si>
   <si>
@@ -277,13 +274,37 @@
   </si>
   <si>
     <t>{d.Region[i].BroodsInspected}</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Inspector</t>
+  </si>
+  <si>
+    <t>{d.Licence[i].Inspector}</t>
+  </si>
+  <si>
+    <t>{d.Licence[i].Other}</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>{d.Licence[i].Region}</t>
+  </si>
+  <si>
+    <t>{d.Licence[i+1].Region}</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +323,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -336,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,12 +383,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -371,10 +394,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,9 +413,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -433,7 +453,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -539,7 +559,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -681,7 +701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -689,44 +709,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B4FD09-964A-4163-B64E-5BD98D9AE9F8}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView zoomScale="159" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="26" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C1" s="4"/>
-      <c r="E1" s="4"/>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="D1" s="4"/>
       <c r="F1" s="4"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -734,189 +755,212 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="S1" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="4"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="4"/>
+      <c r="H2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="2"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="Q2" s="4"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="D5" s="12"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="G6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="H6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L6" s="5" t="s">
+      <c r="M6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="5" t="s">
+      <c r="P6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="R6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="5" t="s">
+      <c r="S6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="5" t="s">
+      <c r="T6" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="U6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="V6" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="D7" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="M7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="N7" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="O7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="O7" s="14" t="s">
+      <c r="P7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="P7" s="14" t="s">
+      <c r="Q7" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="Q7" s="14" t="s">
+      <c r="R7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="R7" s="14" t="s">
+      <c r="S7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="S7" s="14" t="s">
+      <c r="T7" s="11" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>50</v>
-      </c>
+      <c r="U7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -927,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB249F7-276C-4CD0-823C-DE856519B24C}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="H1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,46 +991,46 @@
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
       <c r="M1" s="1"/>
       <c r="N1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="O1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="9" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
       <c r="M2" s="1"/>
       <c r="N2" s="2"/>
     </row>
@@ -1012,7 +1056,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>6</v>
@@ -1047,130 +1091,116 @@
       <c r="N6" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="C7" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D7" s="14" t="s">
+      <c r="E7" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="G7" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="I7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="J7" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="K7" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="L7" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="M7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="N7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="N7" s="14" t="s">
+      <c r="O7" s="11"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-    </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1180,6 +1210,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B8CBF3948AF16E4A9427EB9CB0C3AFDB" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fc8a81a77eeb73bda9729b3f784b8c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc8b8595-9fa1-49bc-a016-2621e7bde64e" xmlns:ns3="e1c8ebbc-f196-4c28-98e9-1900bd408e79" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="88ad40c7f0e134defa4acd5e486d3459" ns2:_="" ns3:_="">
     <xsd:import namespace="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
@@ -1390,7 +1426,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1399,13 +1435,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8385E0-3C6B-44E0-B051-89C807FA11B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{710596F7-33DB-499C-9202-13CC66DA1061}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1424,27 +1471,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D213D4AC-AA3E-4F07-BD45-2E303A245682}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D8385E0-3C6B-44E0-B051-89C807FA11B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e1c8ebbc-f196-4c28-98e9-1900bd408e79"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bc8b8595-9fa1-49bc-a016-2621e7bde64e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>